<commit_message>
25-02-2025_Correctly gets series and parallel no.
</commit_message>
<xml_diff>
--- a/Battery database from open source_CellDatabase_v6.xlsx
+++ b/Battery database from open source_CellDatabase_v6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://computingservices-my.sharepoint.com/personal/ojb56_bath_ac_uk/Documents/4th Year/Semester 2/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC68786B-84FA-4A6B-A7FB-5A7B9F03448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{CC68786B-84FA-4A6B-A7FB-5A7B9F03448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{846C15BF-E710-4963-8947-A1D2F954D546}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5111,7 +5111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -5189,23 +5189,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5216,12 +5214,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -49225,83 +49218,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A172DD6-C11B-4857-88C4-0584815F29E6}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.21875" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.77734375" style="37" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" style="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.21875" style="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.21875" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="37"/>
+    <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="1" t="s">
         <v>1475</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>1476</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>1477</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>1478</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>1479</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>1480</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>1481</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>1482</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>1483</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="1" t="s">
         <v>1484</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="D2" s="36" t="s">
+      <c r="B2" s="35"/>
+      <c r="D2" s="35" t="s">
         <v>1485</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="35" t="s">
         <v>1486</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="35" t="s">
         <v>1487</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="35" t="s">
         <v>1488</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="35" t="s">
         <v>1489</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:10" s="32" customFormat="1">
       <c r="A4" s="32" t="s">
@@ -49319,19 +49311,19 @@
       <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="37" t="s">
+      <c r="A5" t="s">
         <v>1492</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="36" t="s">
         <v>1493</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="36">
         <v>3.38</v>
       </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:10" s="32" customFormat="1">
       <c r="A6" s="32" t="s">
@@ -49347,17 +49339,17 @@
       <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="37" t="s">
+      <c r="A7" t="s">
         <v>1495</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="D7" s="38">
+      <c r="B7" s="36"/>
+      <c r="D7" s="36">
         <v>0.3</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
     </row>
     <row r="8" spans="1:10" s="32" customFormat="1">
       <c r="A8" s="32" t="s">
@@ -49366,7 +49358,7 @@
       <c r="B8" s="33" t="s">
         <v>1497</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="42">
         <v>505</v>
       </c>
       <c r="E8" s="32">
@@ -49389,31 +49381,31 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="37" t="s">
+      <c r="A9" t="s">
         <v>1498</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="36" t="s">
         <v>1499</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="37">
         <v>135000</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9">
         <v>97000</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9">
         <v>74600</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9">
         <v>27700</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9">
         <v>49800</v>
       </c>
-      <c r="I9" s="37">
+      <c r="I9">
         <v>107000</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9">
         <v>45000</v>
       </c>
     </row>
@@ -49424,54 +49416,54 @@
       <c r="B10" s="33" t="s">
         <v>1501</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="43">
         <v>177</v>
       </c>
       <c r="E10" s="32">
         <v>169</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="43">
         <v>162</v>
       </c>
-      <c r="G10" s="45">
+      <c r="G10" s="43">
         <v>97.8</v>
       </c>
       <c r="H10" s="32">
         <v>125</v>
       </c>
-      <c r="I10" s="45">
+      <c r="I10" s="43">
         <v>167</v>
       </c>
-      <c r="J10" s="45">
+      <c r="J10" s="43">
         <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="37" t="s">
+      <c r="A11" t="s">
         <v>1502</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="36" t="s">
         <v>1503</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="38">
         <v>30</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11">
         <v>18</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="38">
         <v>29</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="38">
         <v>30</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11">
         <v>24</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11">
         <v>320</v>
       </c>
-      <c r="J11" s="37">
+      <c r="J11">
         <v>52</v>
       </c>
     </row>
@@ -49482,30 +49474,30 @@
       <c r="B12" s="33" t="s">
         <v>1499</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
+      <c r="D12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="37" t="s">
+      <c r="A13" t="s">
         <v>1505</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="36" t="s">
         <v>1506</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="38">
         <v>11</v>
       </c>
-      <c r="E13" s="37">
+      <c r="E13">
         <v>11</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="38">
         <v>11</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="38">
         <v>7.5</v>
       </c>
-      <c r="H13" s="37">
+      <c r="H13">
         <v>6.25</v>
       </c>
     </row>
@@ -49516,16 +49508,16 @@
       <c r="B14" s="33" t="s">
         <v>1508</v>
       </c>
-      <c r="D14" s="46">
-        <v>562000</v>
+      <c r="D14" s="44">
+        <v>496000</v>
       </c>
       <c r="E14" s="32">
         <v>736000</v>
       </c>
-      <c r="F14" s="45">
+      <c r="F14" s="43">
         <v>239000</v>
       </c>
-      <c r="G14" s="45">
+      <c r="G14" s="43">
         <v>90000</v>
       </c>
       <c r="H14" s="32">
@@ -49539,31 +49531,31 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="37" t="s">
+      <c r="A15" t="s">
         <v>1509</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="36" t="s">
         <v>1508</v>
       </c>
-      <c r="D15" s="39">
+      <c r="D15" s="37">
         <v>210000</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E15">
         <v>320000</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="38">
         <v>188000</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="38">
         <v>50000</v>
       </c>
-      <c r="H15" s="37">
+      <c r="H15">
         <v>170000</v>
       </c>
-      <c r="I15" s="37">
+      <c r="I15">
         <v>250000</v>
       </c>
-      <c r="J15" s="37">
+      <c r="J15">
         <v>50000</v>
       </c>
     </row>
@@ -49574,16 +49566,16 @@
       <c r="B16" s="33" t="s">
         <v>1508</v>
       </c>
-      <c r="D16" s="46">
+      <c r="D16" s="44">
         <v>11500</v>
       </c>
       <c r="E16" s="32">
         <v>11000</v>
       </c>
-      <c r="F16" s="45">
+      <c r="F16" s="43">
         <v>7000</v>
       </c>
-      <c r="G16" s="45">
+      <c r="G16" s="43">
         <v>6600</v>
       </c>
       <c r="H16" s="32">
@@ -49591,15 +49583,15 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="37" t="s">
+      <c r="A17" t="s">
         <v>1511</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="36" t="s">
         <v>1508</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
+      <c r="D17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="1:10" s="32" customFormat="1">
       <c r="A18" s="32" t="s">
@@ -49608,36 +49600,36 @@
       <c r="B18" s="33" t="s">
         <v>1513</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
+      <c r="D18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="37" t="s">
+      <c r="A19" t="s">
         <v>1514</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="36" t="s">
         <v>1491</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="38">
         <v>795.92</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19">
         <v>621</v>
       </c>
-      <c r="F19" s="40">
+      <c r="F19" s="38">
         <v>477.1</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="38">
         <v>315</v>
       </c>
-      <c r="H19" s="37">
+      <c r="H19">
         <v>438</v>
       </c>
-      <c r="I19" s="40">
+      <c r="I19" s="38">
         <v>664.7</v>
       </c>
-      <c r="J19" s="40">
+      <c r="J19" s="38">
         <v>415</v>
       </c>
     </row>
@@ -49648,13 +49640,13 @@
       <c r="B20" s="33" t="s">
         <v>1491</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="43">
         <v>540</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="43">
         <v>331.2</v>
       </c>
-      <c r="G20" s="45">
+      <c r="G20" s="43">
         <v>185.5</v>
       </c>
       <c r="H20" s="32">
@@ -49665,28 +49657,28 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="37" t="s">
+      <c r="A21" t="s">
         <v>1516</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="36" t="s">
         <v>1517</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="38">
         <v>360</v>
       </c>
-      <c r="F21" s="40">
+      <c r="F21" s="38">
         <v>111.11</v>
       </c>
-      <c r="G21" s="40">
+      <c r="G21" s="38">
         <v>86</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21">
         <v>163.30000000000001</v>
       </c>
-      <c r="I21" s="40">
+      <c r="I21" s="38">
         <v>296</v>
       </c>
-      <c r="J21" s="40">
+      <c r="J21" s="38">
         <v>153</v>
       </c>
     </row>
@@ -49697,13 +49689,13 @@
       <c r="B22" s="33" t="s">
         <v>1519</v>
       </c>
-      <c r="D22" s="45">
+      <c r="D22" s="43">
         <v>459</v>
       </c>
-      <c r="F22" s="45">
+      <c r="F22" s="43">
         <v>806</v>
       </c>
-      <c r="G22" s="45">
+      <c r="G22" s="43">
         <v>398</v>
       </c>
       <c r="J22" s="32">
@@ -49711,19 +49703,19 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="37" t="s">
+      <c r="A23" t="s">
         <v>1520</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="38">
         <v>216</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F23" s="38">
         <v>480</v>
       </c>
-      <c r="G23" s="40">
+      <c r="G23" s="38">
         <v>240</v>
       </c>
     </row>
@@ -49734,10 +49726,10 @@
       <c r="B24" s="33" t="s">
         <v>1519</v>
       </c>
-      <c r="F24" s="45">
+      <c r="F24" s="43">
         <v>697</v>
       </c>
-      <c r="G24" s="45">
+      <c r="G24" s="43">
         <v>360</v>
       </c>
       <c r="H24" s="32">
@@ -49751,40 +49743,40 @@
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="B25" s="38"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
+      <c r="B25" s="36"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="1" t="s">
         <v>1522</v>
       </c>
-      <c r="B26" s="38"/>
+      <c r="B26" s="36"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="37" t="s">
+      <c r="A27" t="s">
         <v>1523</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="D27" s="41">
+      <c r="B27" s="36"/>
+      <c r="D27" s="39">
         <v>7776</v>
       </c>
-      <c r="E27" s="37">
+      <c r="E27">
         <v>396</v>
       </c>
-      <c r="F27" s="40">
+      <c r="F27" s="38">
         <v>384</v>
       </c>
-      <c r="G27" s="40">
+      <c r="G27" s="38">
         <v>192</v>
       </c>
-      <c r="H27" s="37">
+      <c r="H27">
         <v>106</v>
       </c>
-      <c r="I27" s="37">
+      <c r="I27">
         <v>204</v>
       </c>
-      <c r="J27" s="37">
+      <c r="J27">
         <v>288</v>
       </c>
     </row>
@@ -49793,7 +49785,7 @@
         <v>1524</v>
       </c>
       <c r="B28" s="33"/>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="45" t="s">
         <v>1525</v>
       </c>
       <c r="E28" s="32" t="s">
@@ -49816,14 +49808,14 @@
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="37" t="s">
+      <c r="A29" t="s">
         <v>1532</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="D29" s="37">
+      <c r="B29" s="36"/>
+      <c r="D29">
         <v>21700</v>
       </c>
-      <c r="H29" s="37" t="s">
+      <c r="H29" t="s">
         <v>1533</v>
       </c>
     </row>
@@ -49849,25 +49841,25 @@
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="37" t="s">
+      <c r="A31" t="s">
         <v>1538</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="D31" s="37">
+      <c r="D31">
         <v>4.2</v>
       </c>
-      <c r="F31" s="37">
+      <c r="F31">
         <v>4.2</v>
       </c>
-      <c r="G31" s="37">
+      <c r="G31">
         <v>4.1500000000000004</v>
       </c>
-      <c r="H31" s="37">
+      <c r="H31">
         <v>3.65</v>
       </c>
-      <c r="I31" s="37">
+      <c r="I31">
         <v>4.2</v>
       </c>
     </row>
@@ -49898,25 +49890,25 @@
       </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="37" t="s">
+      <c r="A33" t="s">
         <v>1540</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="36" t="s">
         <v>1519</v>
       </c>
-      <c r="D33" s="37">
+      <c r="D33">
         <v>2.5</v>
       </c>
-      <c r="F33" s="48">
+      <c r="F33">
         <v>2.5</v>
       </c>
-      <c r="G33" s="48">
+      <c r="G33">
         <v>2.5</v>
       </c>
-      <c r="H33" s="48">
+      <c r="H33">
         <v>2.5</v>
       </c>
-      <c r="I33" s="37">
+      <c r="I33">
         <v>2.5</v>
       </c>
     </row>
@@ -49930,13 +49922,13 @@
       <c r="D34" s="32">
         <v>5</v>
       </c>
-      <c r="F34" s="51">
+      <c r="F34" s="46">
         <v>55.6</v>
       </c>
-      <c r="G34" s="51">
+      <c r="G34" s="46">
         <v>43</v>
       </c>
-      <c r="H34" s="49">
+      <c r="H34" s="32">
         <v>161</v>
       </c>
       <c r="I34" s="32">
@@ -49947,30 +49939,30 @@
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="37" t="s">
+      <c r="A35" t="s">
         <v>1542</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="36" t="s">
         <v>1499</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="40">
         <f>D34*D32</f>
         <v>18</v>
       </c>
-      <c r="F35" s="50">
+      <c r="F35" s="38">
         <v>201.8</v>
       </c>
-      <c r="G35" s="42">
+      <c r="G35" s="40">
         <f>G34*G32</f>
         <v>160.38999999999999</v>
       </c>
-      <c r="H35" s="48">
+      <c r="H35">
         <v>515</v>
       </c>
-      <c r="I35" s="37">
+      <c r="I35">
         <v>544</v>
       </c>
-      <c r="J35" s="37">
+      <c r="J35">
         <v>188.7</v>
       </c>
     </row>
@@ -49984,22 +49976,22 @@
       <c r="D36" s="32">
         <v>9.8000000000000007</v>
       </c>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
       <c r="H36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="37" t="s">
+      <c r="A37" t="s">
         <v>1545</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="36" t="s">
         <v>1544</v>
       </c>
-      <c r="D37" s="37">
+      <c r="D37">
         <v>4.7530000000000001</v>
       </c>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
     </row>
     <row r="38" spans="1:10" s="32" customFormat="1">
       <c r="A38" s="32" t="s">
@@ -50011,24 +50003,24 @@
       <c r="D38" s="32">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45">
+      <c r="F38" s="43"/>
+      <c r="G38" s="43">
         <v>41</v>
       </c>
       <c r="H38" s="34"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="37" t="s">
+      <c r="A39" t="s">
         <v>1547</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="36" t="s">
         <v>1544</v>
       </c>
-      <c r="D39" s="37">
+      <c r="D39">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40">
+      <c r="F39" s="38"/>
+      <c r="G39" s="38">
         <v>55</v>
       </c>
     </row>
@@ -50042,18 +50034,18 @@
       <c r="D40" s="32">
         <v>2.4500000000000002</v>
       </c>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45">
+      <c r="F40" s="43"/>
+      <c r="G40" s="43">
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15">
-      <c r="A41" s="37" t="s">
+      <c r="A41" t="s">
         <v>1549</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="43" t="s">
+      <c r="B41" s="36"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="41" t="s">
         <v>1550</v>
       </c>
     </row>
@@ -50064,10 +50056,10 @@
       <c r="B42" s="33" t="s">
         <v>1501</v>
       </c>
-      <c r="F42" s="45">
+      <c r="F42" s="43">
         <v>234</v>
       </c>
-      <c r="G42" s="45">
+      <c r="G42" s="43">
         <v>166</v>
       </c>
       <c r="J42" s="32">

</xml_diff>

<commit_message>
25-02-2025_Series parallel config function
</commit_message>
<xml_diff>
--- a/Battery database from open source_CellDatabase_v6.xlsx
+++ b/Battery database from open source_CellDatabase_v6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://computingservices-my.sharepoint.com/personal/ojb56_bath_ac_uk/Documents/4th Year/Semester 2/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{CC68786B-84FA-4A6B-A7FB-5A7B9F03448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{846C15BF-E710-4963-8947-A1D2F954D546}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{CC68786B-84FA-4A6B-A7FB-5A7B9F03448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEB43655-BF56-4A43-9B01-1744B1CE3F4B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49218,8 +49218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A172DD6-C11B-4857-88C4-0584815F29E6}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -49862,6 +49862,9 @@
       <c r="I31">
         <v>4.2</v>
       </c>
+      <c r="J31">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="32" spans="1:10" s="32" customFormat="1">
       <c r="A32" s="32" t="s">
@@ -49909,6 +49912,9 @@
         <v>2.5</v>
       </c>
       <c r="I33">
+        <v>2.5</v>
+      </c>
+      <c r="J33">
         <v>2.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
25-02-2025_Series parallel function modified
</commit_message>
<xml_diff>
--- a/Battery database from open source_CellDatabase_v6.xlsx
+++ b/Battery database from open source_CellDatabase_v6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://computingservices-my.sharepoint.com/personal/ojb56_bath_ac_uk/Documents/4th Year/Semester 2/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{CC68786B-84FA-4A6B-A7FB-5A7B9F03448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEB43655-BF56-4A43-9B01-1744B1CE3F4B}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{CC68786B-84FA-4A6B-A7FB-5A7B9F03448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18E919C1-2FFA-4C47-A546-72771E6DBB7F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7143" uniqueCount="1552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7145" uniqueCount="1554">
   <si>
     <t>x</t>
   </si>
@@ -4871,12 +4871,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>rated discharge capacity</t>
-  </si>
-  <si>
-    <t>standard discharge capacity</t>
-  </si>
-  <si>
     <t xml:space="preserve">max charge current </t>
   </si>
   <si>
@@ -4890,6 +4884,18 @@
   </si>
   <si>
     <t>Gravemetric energy density</t>
+  </si>
+  <si>
+    <t>standard discharge current</t>
+  </si>
+  <si>
+    <t>Peak power</t>
+  </si>
+  <si>
+    <t>Voltage for peak power</t>
+  </si>
+  <si>
+    <t>Range plus LFP</t>
   </si>
 </sst>
 </file>
@@ -4899,7 +4905,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5051,6 +5057,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -5111,7 +5124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -5203,7 +5216,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5217,6 +5229,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -49216,10 +49233,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A172DD6-C11B-4857-88C4-0584815F29E6}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -49227,7 +49244,7 @@
     <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.77734375" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
@@ -49293,7 +49310,9 @@
       <c r="E3" s="35"/>
       <c r="F3" s="35"/>
       <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="H3" s="35" t="s">
+        <v>1553</v>
+      </c>
     </row>
     <row r="4" spans="1:10" s="32" customFormat="1">
       <c r="A4" s="32" t="s">
@@ -49358,7 +49377,7 @@
       <c r="B8" s="33" t="s">
         <v>1497</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="41">
         <v>505</v>
       </c>
       <c r="E8" s="32">
@@ -49416,25 +49435,25 @@
       <c r="B10" s="33" t="s">
         <v>1501</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="42">
         <v>177</v>
       </c>
       <c r="E10" s="32">
         <v>169</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="42">
         <v>162</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="42">
         <v>97.8</v>
       </c>
       <c r="H10" s="32">
         <v>125</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="42">
         <v>167</v>
       </c>
-      <c r="J10" s="43">
+      <c r="J10" s="42">
         <v>131</v>
       </c>
     </row>
@@ -49474,9 +49493,9 @@
       <c r="B12" s="33" t="s">
         <v>1499</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="D12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
@@ -49508,16 +49527,16 @@
       <c r="B14" s="33" t="s">
         <v>1508</v>
       </c>
-      <c r="D14" s="44">
-        <v>496000</v>
+      <c r="D14" s="43">
+        <v>511000</v>
       </c>
       <c r="E14" s="32">
         <v>736000</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="42">
         <v>239000</v>
       </c>
-      <c r="G14" s="43">
+      <c r="G14" s="42">
         <v>90000</v>
       </c>
       <c r="H14" s="32">
@@ -49566,16 +49585,16 @@
       <c r="B16" s="33" t="s">
         <v>1508</v>
       </c>
-      <c r="D16" s="44">
+      <c r="D16" s="43">
         <v>11500</v>
       </c>
       <c r="E16" s="32">
         <v>11000</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="42">
         <v>7000</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="42">
         <v>6600</v>
       </c>
       <c r="H16" s="32">
@@ -49600,9 +49619,9 @@
       <c r="B18" s="33" t="s">
         <v>1513</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="D18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
@@ -49640,13 +49659,13 @@
       <c r="B20" s="33" t="s">
         <v>1491</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="42">
         <v>540</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="42">
         <v>331.2</v>
       </c>
-      <c r="G20" s="43">
+      <c r="G20" s="42">
         <v>185.5</v>
       </c>
       <c r="H20" s="32">
@@ -49689,14 +49708,17 @@
       <c r="B22" s="33" t="s">
         <v>1519</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="42">
         <v>459</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="42">
         <v>806</v>
       </c>
-      <c r="G22" s="43">
+      <c r="G22" s="42">
         <v>398</v>
+      </c>
+      <c r="H22" s="32">
+        <v>400</v>
       </c>
       <c r="J22" s="32">
         <v>500</v>
@@ -49718,6 +49740,9 @@
       <c r="G23" s="38">
         <v>240</v>
       </c>
+      <c r="H23" s="47">
+        <v>265</v>
+      </c>
     </row>
     <row r="24" spans="1:10" s="32" customFormat="1">
       <c r="A24" s="32" t="s">
@@ -49726,10 +49751,10 @@
       <c r="B24" s="33" t="s">
         <v>1519</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="42">
         <v>697</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="42">
         <v>360</v>
       </c>
       <c r="H24" s="32">
@@ -49785,7 +49810,7 @@
         <v>1524</v>
       </c>
       <c r="B28" s="33"/>
-      <c r="D28" s="45" t="s">
+      <c r="D28" s="44" t="s">
         <v>1525</v>
       </c>
       <c r="E28" s="32" t="s">
@@ -49833,6 +49858,9 @@
       <c r="G30" s="32" t="s">
         <v>1536</v>
       </c>
+      <c r="H30" s="32" t="s">
+        <v>1537</v>
+      </c>
       <c r="I30" s="32" t="s">
         <v>1537</v>
       </c>
@@ -49928,10 +49956,10 @@
       <c r="D34" s="32">
         <v>5</v>
       </c>
-      <c r="F34" s="46">
+      <c r="F34" s="45">
         <v>55.6</v>
       </c>
-      <c r="G34" s="46">
+      <c r="G34" s="45">
         <v>43</v>
       </c>
       <c r="H34" s="32">
@@ -49980,28 +50008,35 @@
         <v>1544</v>
       </c>
       <c r="D36" s="32">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="34"/>
+        <v>18.5</v>
+      </c>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="44">
+        <v>782</v>
+      </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>1545</v>
+        <v>1550</v>
       </c>
       <c r="B37" s="36" t="s">
         <v>1544</v>
       </c>
       <c r="D37">
-        <v>4.7530000000000001</v>
+        <v>7.61</v>
       </c>
       <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
+      <c r="G37" s="38">
+        <v>41</v>
+      </c>
+      <c r="H37" s="39">
+        <v>297</v>
+      </c>
     </row>
     <row r="38" spans="1:10" s="32" customFormat="1">
       <c r="A38" s="32" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="B38" s="33" t="s">
         <v>1544</v>
@@ -50009,67 +50044,79 @@
       <c r="D38" s="32">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43">
-        <v>41</v>
-      </c>
-      <c r="H38" s="34"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42">
+        <v>55</v>
+      </c>
+      <c r="I38" s="34">
+        <f>2.25*148</f>
+        <v>333</v>
+      </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>1544</v>
       </c>
       <c r="D39">
-        <v>4.9000000000000004</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="F39" s="38"/>
       <c r="G39" s="38">
-        <v>55</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="32" customFormat="1">
+    <row r="40" spans="1:10" s="32" customFormat="1" ht="15">
       <c r="A40" s="32" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="46" t="s">
         <v>1548</v>
       </c>
-      <c r="B40" s="33" t="s">
-        <v>1544</v>
-      </c>
-      <c r="D40" s="32">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43">
-        <v>12</v>
-      </c>
     </row>
-    <row r="41" spans="1:10" ht="15">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>1549</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="41" t="s">
-        <v>1550</v>
+      <c r="B41" s="36" t="s">
+        <v>1501</v>
+      </c>
+      <c r="F41" s="38">
+        <v>234</v>
+      </c>
+      <c r="G41" s="38">
+        <v>166</v>
+      </c>
+      <c r="J41">
+        <v>213</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="32" customFormat="1">
+    <row r="42" spans="1:10">
       <c r="A42" s="32" t="s">
         <v>1551</v>
       </c>
-      <c r="B42" s="33" t="s">
-        <v>1501</v>
-      </c>
-      <c r="F42" s="43">
-        <v>234</v>
-      </c>
-      <c r="G42" s="43">
-        <v>166</v>
-      </c>
-      <c r="J42" s="32">
-        <v>213</v>
+      <c r="D42" s="32">
+        <v>65.8</v>
+      </c>
+      <c r="H42">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" t="s">
+        <v>1552</v>
+      </c>
+      <c r="D43" s="48">
+        <f>D42/D36</f>
+        <v>3.5567567567567564</v>
+      </c>
+      <c r="H43" s="48">
+        <f>H42/H36</f>
+        <v>2.8644501278772379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
26-02-25 Range-estimation and s-p config update
</commit_message>
<xml_diff>
--- a/Battery database from open source_CellDatabase_v6.xlsx
+++ b/Battery database from open source_CellDatabase_v6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://computingservices-my.sharepoint.com/personal/ojb56_bath_ac_uk/Documents/4th Year/Semester 2/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{CC68786B-84FA-4A6B-A7FB-5A7B9F03448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18E919C1-2FFA-4C47-A546-72771E6DBB7F}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{CC68786B-84FA-4A6B-A7FB-5A7B9F03448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF1F6E7A-A4BB-437E-BEEC-B40655DF3617}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW DATA" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7145" uniqueCount="1554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7148" uniqueCount="1557">
   <si>
     <t>x</t>
   </si>
@@ -4896,6 +4896,15 @@
   </si>
   <si>
     <t>Range plus LFP</t>
+  </si>
+  <si>
+    <t>Kia Niro</t>
+  </si>
+  <si>
+    <t>crossover SUV</t>
+  </si>
+  <si>
+    <t>98s 3p</t>
   </si>
 </sst>
 </file>
@@ -5059,7 +5068,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF0070C0"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5124,7 +5133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -5230,10 +5239,11 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -49233,10 +49243,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A172DD6-C11B-4857-88C4-0584815F29E6}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -49253,7 +49263,7 @@
     <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>1475</v>
       </c>
@@ -49281,8 +49291,11 @@
       <c r="J1" s="35" t="s">
         <v>1483</v>
       </c>
+      <c r="K1" s="35" t="s">
+        <v>1554</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>1484</v>
       </c>
@@ -49302,19 +49315,27 @@
       <c r="H2" s="35" t="s">
         <v>1489</v>
       </c>
+      <c r="K2" s="35" t="s">
+        <v>1555</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="1"/>
       <c r="B3" s="35"/>
       <c r="D3" s="35"/>
       <c r="E3" s="35"/>
       <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="G3" s="35">
+        <v>2015</v>
+      </c>
       <c r="H3" s="35" t="s">
         <v>1553</v>
       </c>
+      <c r="K3">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" s="32" customFormat="1">
+    <row r="4" spans="1:11" s="32" customFormat="1">
       <c r="A4" s="32" t="s">
         <v>1490</v>
       </c>
@@ -49329,7 +49350,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>1492</v>
       </c>
@@ -49344,7 +49365,7 @@
       <c r="G5" s="36"/>
       <c r="H5" s="36"/>
     </row>
-    <row r="6" spans="1:10" s="32" customFormat="1">
+    <row r="6" spans="1:11" s="32" customFormat="1">
       <c r="A6" s="32" t="s">
         <v>1494</v>
       </c>
@@ -49357,7 +49378,7 @@
       <c r="G6" s="33"/>
       <c r="H6" s="33"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>1495</v>
       </c>
@@ -49370,7 +49391,7 @@
       <c r="G7" s="36"/>
       <c r="H7" s="36"/>
     </row>
-    <row r="8" spans="1:10" s="32" customFormat="1">
+    <row r="8" spans="1:11" s="32" customFormat="1">
       <c r="A8" s="32" t="s">
         <v>1496</v>
       </c>
@@ -49399,7 +49420,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>1498</v>
       </c>
@@ -49427,8 +49448,11 @@
       <c r="J9">
         <v>45000</v>
       </c>
+      <c r="K9">
+        <v>68000</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" s="32" customFormat="1">
+    <row r="10" spans="1:11" s="32" customFormat="1">
       <c r="A10" s="32" t="s">
         <v>1500</v>
       </c>
@@ -49456,8 +49480,11 @@
       <c r="J10" s="42">
         <v>131</v>
       </c>
+      <c r="K10" s="32">
+        <v>154</v>
+      </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>1502</v>
       </c>
@@ -49485,8 +49512,11 @@
       <c r="J11">
         <v>52</v>
       </c>
+      <c r="K11">
+        <v>44</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" s="32" customFormat="1">
+    <row r="12" spans="1:11" s="32" customFormat="1">
       <c r="A12" s="32" t="s">
         <v>1504</v>
       </c>
@@ -49497,7 +49527,7 @@
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>1505</v>
       </c>
@@ -49520,7 +49550,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="32" customFormat="1">
+    <row r="14" spans="1:11" s="32" customFormat="1">
       <c r="A14" s="32" t="s">
         <v>1507</v>
       </c>
@@ -49548,8 +49578,11 @@
       <c r="J14" s="32">
         <v>167000</v>
       </c>
+      <c r="K14" s="32">
+        <v>150000</v>
+      </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>1509</v>
       </c>
@@ -49577,8 +49610,11 @@
       <c r="J15">
         <v>50000</v>
       </c>
+      <c r="K15">
+        <v>77000</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" s="32" customFormat="1">
+    <row r="16" spans="1:11" s="32" customFormat="1">
       <c r="A16" s="32" t="s">
         <v>1510</v>
       </c>
@@ -49601,7 +49637,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>1511</v>
       </c>
@@ -49612,7 +49648,7 @@
       <c r="F17" s="38"/>
       <c r="G17" s="38"/>
     </row>
-    <row r="18" spans="1:10" s="32" customFormat="1">
+    <row r="18" spans="1:11" s="32" customFormat="1">
       <c r="A18" s="32" t="s">
         <v>1512</v>
       </c>
@@ -49623,7 +49659,7 @@
       <c r="F18" s="42"/>
       <c r="G18" s="42"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>1514</v>
       </c>
@@ -49651,8 +49687,11 @@
       <c r="J19" s="38">
         <v>415</v>
       </c>
+      <c r="K19" s="38">
+        <v>443</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" s="32" customFormat="1">
+    <row r="20" spans="1:11" s="32" customFormat="1">
       <c r="A20" s="32" t="s">
         <v>1515</v>
       </c>
@@ -49674,8 +49713,11 @@
       <c r="J20" s="32">
         <v>255</v>
       </c>
+      <c r="K20" s="32">
+        <v>264</v>
+      </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>1516</v>
       </c>
@@ -49700,8 +49742,11 @@
       <c r="J21" s="38">
         <v>153</v>
       </c>
+      <c r="K21" s="38">
+        <v>180.9</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" s="32" customFormat="1">
+    <row r="22" spans="1:11" s="32" customFormat="1">
       <c r="A22" s="32" t="s">
         <v>1518</v>
       </c>
@@ -49723,8 +49768,11 @@
       <c r="J22" s="32">
         <v>500</v>
       </c>
+      <c r="K22" s="48">
+        <v>450</v>
+      </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>1520</v>
       </c>
@@ -49740,11 +49788,14 @@
       <c r="G23" s="38">
         <v>240</v>
       </c>
-      <c r="H23" s="47">
+      <c r="H23" s="49">
         <v>265</v>
       </c>
+      <c r="K23" s="49">
+        <v>245</v>
+      </c>
     </row>
-    <row r="24" spans="1:10" s="32" customFormat="1">
+    <row r="24" spans="1:11" s="32" customFormat="1">
       <c r="A24" s="32" t="s">
         <v>1521</v>
       </c>
@@ -49766,19 +49817,22 @@
       <c r="J24" s="32">
         <v>355.2</v>
       </c>
+      <c r="K24" s="32">
+        <v>356</v>
+      </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:11">
       <c r="B25" s="36"/>
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
         <v>1522</v>
       </c>
       <c r="B26" s="36"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>1523</v>
       </c>
@@ -49804,8 +49858,11 @@
       <c r="J27">
         <v>288</v>
       </c>
+      <c r="K27">
+        <v>294</v>
+      </c>
     </row>
-    <row r="28" spans="1:10" s="32" customFormat="1">
+    <row r="28" spans="1:11" s="32" customFormat="1">
       <c r="A28" s="32" t="s">
         <v>1524</v>
       </c>
@@ -49831,8 +49888,11 @@
       <c r="J28" s="32" t="s">
         <v>1531</v>
       </c>
+      <c r="K28" s="32" t="s">
+        <v>1556</v>
+      </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>1532</v>
       </c>
@@ -49844,7 +49904,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="32" customFormat="1">
+    <row r="30" spans="1:11" s="32" customFormat="1">
       <c r="A30" s="32" t="s">
         <v>1534</v>
       </c>
@@ -49868,7 +49928,7 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>1538</v>
       </c>
@@ -49893,8 +49953,11 @@
       <c r="J31">
         <v>4.2</v>
       </c>
+      <c r="K31">
+        <v>4.2</v>
+      </c>
     </row>
-    <row r="32" spans="1:10" s="32" customFormat="1">
+    <row r="32" spans="1:11" s="32" customFormat="1">
       <c r="A32" s="32" t="s">
         <v>1539</v>
       </c>
@@ -49919,8 +49982,11 @@
       <c r="J32" s="32">
         <v>3.7</v>
       </c>
+      <c r="K32" s="32">
+        <v>3.63</v>
+      </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>1540</v>
       </c>
@@ -49945,8 +50011,11 @@
       <c r="J33">
         <v>2.5</v>
       </c>
+      <c r="K33">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="34" spans="1:10" s="32" customFormat="1">
+    <row r="34" spans="1:11" s="32" customFormat="1">
       <c r="A34" s="32" t="s">
         <v>1541</v>
       </c>
@@ -49971,8 +50040,11 @@
       <c r="J34" s="32">
         <v>51</v>
       </c>
+      <c r="K34" s="32">
+        <v>60</v>
+      </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>1542</v>
       </c>
@@ -49999,8 +50071,11 @@
       <c r="J35">
         <v>188.7</v>
       </c>
+      <c r="K35">
+        <v>218</v>
+      </c>
     </row>
-    <row r="36" spans="1:10" s="32" customFormat="1">
+    <row r="36" spans="1:11" s="32" customFormat="1">
       <c r="A36" s="32" t="s">
         <v>1543</v>
       </c>
@@ -50015,8 +50090,11 @@
       <c r="H36" s="44">
         <v>782</v>
       </c>
+      <c r="K36" s="32">
+        <v>284</v>
+      </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>1550</v>
       </c>
@@ -50033,8 +50111,11 @@
       <c r="H37" s="39">
         <v>297</v>
       </c>
+      <c r="K37">
+        <v>120</v>
+      </c>
     </row>
-    <row r="38" spans="1:10" s="32" customFormat="1">
+    <row r="38" spans="1:11" s="32" customFormat="1">
       <c r="A38" s="32" t="s">
         <v>1545</v>
       </c>
@@ -50053,7 +50134,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>1546</v>
       </c>
@@ -50068,7 +50149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="32" customFormat="1" ht="15">
+    <row r="40" spans="1:11" s="32" customFormat="1" ht="15">
       <c r="A40" s="32" t="s">
         <v>1547</v>
       </c>
@@ -50078,7 +50159,7 @@
         <v>1548</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>1549</v>
       </c>
@@ -50094,29 +50175,44 @@
       <c r="J41">
         <v>213</v>
       </c>
+      <c r="K41">
+        <v>242</v>
+      </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:11">
       <c r="A42" s="32" t="s">
         <v>1551</v>
       </c>
       <c r="D42" s="32">
         <v>65.8</v>
       </c>
+      <c r="G42" s="40">
+        <f>G14/G27</f>
+        <v>468.75</v>
+      </c>
       <c r="H42">
         <v>2240</v>
       </c>
+      <c r="K42">
+        <v>968</v>
+      </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>1552</v>
       </c>
-      <c r="D43" s="48">
+      <c r="D43" s="47">
         <f>D42/D36</f>
         <v>3.5567567567567564</v>
       </c>
-      <c r="H43" s="48">
+      <c r="G43" s="47"/>
+      <c r="H43" s="47">
         <f>H42/H36</f>
         <v>2.8644501278772379</v>
+      </c>
+      <c r="K43" s="47">
+        <f>K42/K36</f>
+        <v>3.408450704225352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
18-03 GUI with desired sliders working and refreshin
</commit_message>
<xml_diff>
--- a/Battery database from open source_CellDatabase_v6.xlsx
+++ b/Battery database from open source_CellDatabase_v6.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://computingservices-my.sharepoint.com/personal/ojb56_bath_ac_uk/Documents/4th Year/Semester 2/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{CC68786B-84FA-4A6B-A7FB-5A7B9F03448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{385ADDDD-27FB-4340-B388-A06DAF83247F}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{CC68786B-84FA-4A6B-A7FB-5A7B9F03448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF58227A-ED2B-4EB2-B297-D5D531B0B236}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5376" yWindow="5352" windowWidth="7956" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW DATA" sheetId="1" r:id="rId1"/>
     <sheet name="batteries in dev" sheetId="2" r:id="rId2"/>
     <sheet name="EV Data" sheetId="3" r:id="rId3"/>
     <sheet name="WLTP Acc" sheetId="4" r:id="rId4"/>
+    <sheet name="Test" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'RAW DATA'!$F$2:$F$395</definedName>
@@ -5288,7 +5289,7 @@
   </sheetPr>
   <dimension ref="A1:AO355"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="8" ySplit="2" topLeftCell="AI116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -43540,11 +43541,11 @@
         <v>759</v>
       </c>
       <c r="AN324">
-        <f t="shared" ref="AN324:AN352" si="27">IF(G324="Pouch",1,IF(G324="Prismatic",2,IF(G324="Cylindrical",3,"")))</f>
+        <f t="shared" ref="AN324:AN348" si="27">IF(G324="Pouch",1,IF(G324="Prismatic",2,IF(G324="Cylindrical",3,"")))</f>
         <v>1</v>
       </c>
       <c r="AO324">
-        <f t="shared" ref="AO324:AO359" si="28">IF(AN324=1, 60.25, IF(AN324=2, 60.79, IF(AN324=3, 64.69, 0)))</f>
+        <f t="shared" ref="AO324:AO355" si="28">IF(AN324=1, 60.25, IF(AN324=2, 60.79, IF(AN324=3, 64.69, 0)))</f>
         <v>60.25</v>
       </c>
     </row>
@@ -77489,6 +77490,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06120487-0105-4568-8F1F-1AB261EBD0D3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{377e3d22-4ea1-422d-b0ad-8fcc89406b9e}" enabled="0" method="" siteId="{377e3d22-4ea1-422d-b0ad-8fcc89406b9e}" removed="1"/>

</xml_diff>